<commit_message>
quickfix - strategy headers not being written correctly
</commit_message>
<xml_diff>
--- a/results formatted.xlsx
+++ b/results formatted.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ethan\Documents\GitHub\Image-Smoother\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{430806C1-D2DE-4D80-B872-4BFCECE5575E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013D2B00-9049-4094-8BB1-B01C4B24CDE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results formatted" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>ORDER STATISTIC - QUICK SORT</t>
   </si>
   <si>
     <t>RANGE\SIZES</t>
   </si>
+  <si>
+    <t>ORDER STATISTIC - ITERATIVE SELECTION</t>
+  </si>
+  <si>
+    <t>ORDER STATISTIC - QUICK SELECT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4204,11 +4210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4218,10 +4224,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed naming of charts
</commit_message>
<xml_diff>
--- a/results formatted.xlsx
+++ b/results formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ethan\Documents\GitHub\Image-Smoother\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013D2B00-9049-4094-8BB1-B01C4B24CDE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10229691-261E-4515-AFD1-2206D3AA2542}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,6 +638,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Quick</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1164,7 +1193,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Quick Sort</a:t>
+              <a:t>Iterative Selection</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1675,6 +1704,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Quick Select</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4214,7 +4268,7 @@
   <dimension ref="A2:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>